<commit_message>
Changed counts and if start_page
</commit_message>
<xml_diff>
--- a/tables/data.xlsx
+++ b/tables/data.xlsx
@@ -1,31 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\parser\tables\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2371350-EB18-43EF-8D1D-9BA2BE05A379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="3045" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="2025-02-17" sheetId="1" r:id="rId1"/>
+    <sheet name="2025-02-18" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Цена за м2</t>
+  </si>
+  <si>
+    <t>Координаты</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,25 +86,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -140,9 +134,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -174,27 +168,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -226,27 +202,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -419,18 +377,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>